<commit_message>
Updated the monthly flow with proper group population and chart creation
</commit_message>
<xml_diff>
--- a/Clustering_Output.xlsx
+++ b/Clustering_Output.xlsx
@@ -469,20 +469,20 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>agglomerativeClustering_SpectralEmbedding_BERT5</t>
+          <t>agglomerativeClustering_SpectralEmbedding_BERT6</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.042860860869816e+31</v>
+        <v>8.782187687781431e+30</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6974548876524067</v>
+        <v>0.5054226446462774</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8354888374931433</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
@@ -491,42 +491,42 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>agglomerativeClustering_SpectralEmbedding_BERT4</t>
+          <t>agglomerativeClustering_SpectralEmbedding_BERT7</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5.209406214822625e+30</v>
+        <v>8.351493156420156e+30</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9999999961122179</v>
+        <v>0.206780496129849</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.4173520079007967</v>
+        <v>0.9509581727613843</v>
       </c>
       <c r="F3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>kmeans_SpectralEmbedding_BERT4</t>
+          <t>agglomerativeClustering_SpectralEmbedding_BERT5</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5.209406214822625e+30</v>
+        <v>4.911648493278301e+30</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9999999961122179</v>
+        <v>0.5888765688896752</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4173520079007967</v>
+        <v>0.5592739153265681</v>
       </c>
       <c r="F4" t="n">
         <v>3</v>
@@ -543,7 +543,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -559,31 +559,31 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>kmeans_SpectralEmbedding_BERT4</t>
+          <t>agglomerativeClustering_SpectralEmbedding_BERT5</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>agglomerativeClustering_SpectralEmbedding_BERT4</t>
+          <t>agglomerativeClustering_SpectralEmbedding_BERT6</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>agglomerativeClustering_SpectralEmbedding_BERT5</t>
+          <t>agglomerativeClustering_SpectralEmbedding_BERT7</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x0', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
+          <t>['Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -592,46 +592,46 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>['Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x0', 'Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0x66', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
+          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>['Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0xc', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
+          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
+          <t>['Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -640,174 +640,174 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0xa']</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0xb']</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x0', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
+          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x0', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0xb']</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x0', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
+          <t>['Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0x3d', 'Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0x25', 'LOCK Hard Hang, did not return to idle in 1s']</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x0', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
+          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x0', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0xb']</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x0', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
+          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C13" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
+          <t>['Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0xb', 'Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0x5', 'LOCK Hard Hang, did not return to idle in 1s']</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D14" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
+          <t>['Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
+          <t>['Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
@@ -816,78 +816,78 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
+          <t>['mscod: MCE when CR4.MCE is clear-Error signaled by the core and logged in Ubox. Check the core for more details.', 'mscod: MCE under WFS-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x5', 'Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0x49', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x3', 'Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0x0']</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D17" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
+          <t>['Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x9', 'Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0xb']</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0xa']</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x9', 'Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x9']</t>
+          <t>['Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -896,123 +896,123 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x9', 'Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x9']</t>
         </is>
       </c>
       <c r="B22" t="n">
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
+          <t>['Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0x11', 'Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0x1b', 'LOCK Hard Hang, did not return to idle in 1s']</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C23" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D23" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>['Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0x13', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0x2a']</t>
+          <t>['Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x9', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
         <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>['Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0x29', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
+          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D25" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x9']</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x9']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x0']</t>
         </is>
       </c>
       <c r="B27" t="n">
         <v>3</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0xb']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x0']</t>
         </is>
       </c>
       <c r="B28" t="n">
         <v>3</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x0']</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C29" t="n">
         <v>3</v>
@@ -1024,254 +1024,254 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>['mscod: MCE under WFS-Error signaled by the core and logged in Ubox. Check the core for more details.', 'mscod: MCE when CR4.MCE is clear-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0x1']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x0']</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C30" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x0']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0xb']</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x0', 'Merge Bank11-MSE signaled an MCA to Ubox; Check mc_status of MCA BANKID:11 and  MCA BANK_INDEX:0x0']</t>
+          <t>['mscod: MCE when CR4.MCE is clear-Error signaled by the core and logged in Ubox. Check the core for more details.', 'mscod: MCE when CR4.MCE is clear-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0xb']</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C32" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
+          <t>['Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x5', 'Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0xa', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x4', 'Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0xb']</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>['Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x0']</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C34" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D34" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x0']</t>
         </is>
       </c>
       <c r="B35" t="n">
         <v>3</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
+          <t>['Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0xa']</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x9', 'Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0xc']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0xa']</t>
         </is>
       </c>
       <c r="B37" t="n">
         <v>1</v>
       </c>
       <c r="C37" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x0']</t>
         </is>
       </c>
       <c r="B38" t="n">
         <v>3</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x9', 'Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0xf']</t>
+          <t>['Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0x1f', 'Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0x17', 'LOCK Hard Hang, did not return to idle in 1s']</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C39" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
+          <t>['Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x9', 'Merge Bank5-UPI signaled an MCA to Ubox; Check mc_status of MCA BANKID:5 and  MCA BANK_INDEX:0x1', 'Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0x1f']</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>['Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0x1', 'LOCK Hard Hang, did not return to idle in 1s']</t>
+          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D41" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x0']</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x9']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x0']</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x0', 'Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0x19']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x0']</t>
         </is>
       </c>
       <c r="B44" t="n">
         <v>1</v>
       </c>
       <c r="C44" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>['mscod: SW triple fault shutdown-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
+          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D45" t="n">
         <v>4</v>
@@ -1280,78 +1280,78 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x9']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x0']</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>['mscod: SW triple fault shutdown-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x0']</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>['Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0x0', 'Merge Bank9-LLC0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:9 and  MCA BANK_INDEX:0x7', 'Merge Bank11-MSE signaled an MCA to Ubox; Check mc_status of MCA BANKID:11 and  MCA BANK_INDEX:0x0']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x0']</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>['Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0x17', 'LOCK Hard Hang, did not return to idle in 1s']</t>
+          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0xd']</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D49" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>['LOCK Hard Hang, did not return to idle in 1s']</t>
+          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D50" t="n">
         <v>2</v>
@@ -1360,30 +1360,30 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>['mscod: SW triple fault shutdown-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
+          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x9']</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>['Merge Bank6-Punit signaled an MCA to Ubox; Check mc_status of MCA BANKID:6 and  MCA BANK_INDEX:0x9']</t>
+          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D52" t="n">
         <v>2</v>
@@ -1392,17 +1392,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.', 'Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0x1']</t>
+          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C53" t="n">
         <v>2</v>
       </c>
       <c r="D53" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54">
@@ -1412,44 +1412,76 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D54" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>['Merge Bank13-DDR_MCCHAN0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:13 and  MCA BANK_INDEX:0x0', 'Merge Bank14-DDR_MCCHAN1 signaled an MCA to Ubox; Check mc_status of MCA BANKID:14 and  MCA BANK_INDEX:0x0']</t>
+          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
         </is>
       </c>
       <c r="B55" t="n">
         <v>2</v>
       </c>
       <c r="C55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>['Merge Bank7-CHA0 signaled an MCA to Ubox; Check mc_status of MCA BANKID:7 and  MCA BANK_INDEX:0xa', 'LOCK Hard Hang, did not return to idle in 1s']</t>
+          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D56" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>2</v>
+      </c>
+      <c r="C57" t="n">
+        <v>2</v>
+      </c>
+      <c r="D57" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>['mscod: MCE when MCIP bit is set-Error signaled by the core and logged in Ubox. Check the core for more details.']</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>2</v>
+      </c>
+      <c r="C58" t="n">
+        <v>2</v>
+      </c>
+      <c r="D58" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>